<commit_message>
Relatório e lista de verificação atualizados
</commit_message>
<xml_diff>
--- a/ListaDeVerificacao.xlsx
+++ b/ListaDeVerificacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PUCRS\ES_Orientada_a_Modelos\T1\Revisao_UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF70888-C6C6-4C91-8C8A-FB4EA28AFA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A998C136-3B8C-410B-B9C2-0226FE141AC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0973AC59-7DCE-4B54-BDFC-EC698FEA6706}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Modelo Inclusivo</t>
   </si>
@@ -50,22 +50,37 @@
     <t>OK</t>
   </si>
   <si>
-    <t>As classes possuem nomes adequados</t>
-  </si>
-  <si>
-    <t>Casos de uso cobrem os requisitos do enunciado</t>
-  </si>
-  <si>
-    <t>Os casos de uso possuem decrições adequadas</t>
-  </si>
-  <si>
-    <t>É explicitado que apenas um usuário deve operar o programa</t>
-  </si>
-  <si>
-    <t>Os atributos das classes possuem nomes claros e adequados</t>
-  </si>
-  <si>
-    <t>A classe faz o cálculo do salário conforme descrito no enunciado</t>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>O diagrama de classe utiliza apenas tipos primitivos independentes de plataforma?</t>
+  </si>
+  <si>
+    <t>Casos de uso cobrem os requisitos do enunciado?</t>
+  </si>
+  <si>
+    <t>Os casos de uso possuem decrições adequadas?</t>
+  </si>
+  <si>
+    <t>É explicitado que apenas um usuário deve operar o programa?</t>
+  </si>
+  <si>
+    <t>As classes possuem nomes adequados?</t>
+  </si>
+  <si>
+    <t>Os atributos das classes possuem nomes claros e adequados?</t>
+  </si>
+  <si>
+    <t>A classe faz o cálculo do salário conforme descrito no enunciado?</t>
+  </si>
+  <si>
+    <t>O nome do autor aparece nos diagramas?</t>
+  </si>
+  <si>
+    <t>O trabalho contém os dois diagramas (caso de uso e diagramas de classe)?</t>
+  </si>
+  <si>
+    <t>O trabalho está disponível em repositório do GitHub?</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -215,19 +230,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -268,14 +347,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -618,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CFEC2C7-7E48-47BE-AC84-9317CFE56FB6}">
   <dimension ref="C3:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +767,8 @@
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -637,92 +778,128 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="17"/>
+      <c r="F4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="19"/>
+      <c r="I4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="7" t="s">
+    <row r="7" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="11" t="s">
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="17"/>
+    <row r="9" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:G10">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -732,11 +909,13 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D10">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D10">
+  <conditionalFormatting sqref="J6:J8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>

</xml_diff>